<commit_message>
correct redirect to test output page with excel export
</commit_message>
<xml_diff>
--- a/Export.xlsx
+++ b/Export.xlsx
@@ -407,7 +407,7 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>37</v>
+        <v>56</v>
       </c>
       <c r="B2">
         <v>15</v>
@@ -425,7 +425,7 @@
         <v>7151:31323334</v>
       </c>
       <c r="G2" s="1">
-        <v>44035.33806605324</v>
+        <v>44041.472538229165</v>
       </c>
     </row>
   </sheetData>
@@ -524,7 +524,7 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>21</v>
+        <v>346</v>
       </c>
       <c r="B2">
         <v>9</v>
@@ -581,7 +581,7 @@
         <v>0</v>
       </c>
       <c r="T2">
-        <v>3.39172</v>
+        <v>3.39566</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -596,15 +596,15 @@
         <v>0</v>
       </c>
       <c r="Y2" s="1">
-        <v>44035.33819440972</v>
+        <v>44041.47266554398</v>
       </c>
       <c r="Z2">
-        <v>37</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3">
       <c r="A3">
-        <v>22</v>
+        <v>347</v>
       </c>
       <c r="B3">
         <v>10</v>
@@ -661,7 +661,7 @@
         <v>0</v>
       </c>
       <c r="T3">
-        <v>1.26117</v>
+        <v>1.2619</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -676,15 +676,15 @@
         <v>0</v>
       </c>
       <c r="Y3" s="1">
-        <v>44035.338308796294</v>
+        <v>44041.47277565972</v>
       </c>
       <c r="Z3">
-        <v>37</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4">
       <c r="A4">
-        <v>23</v>
+        <v>348</v>
       </c>
       <c r="B4">
         <v>11</v>
@@ -741,7 +741,7 @@
         <v>0</v>
       </c>
       <c r="T4">
-        <v>0.05559</v>
+        <v>0.05568</v>
       </c>
       <c r="U4">
         <v>0</v>
@@ -756,15 +756,15 @@
         <v>0</v>
       </c>
       <c r="Y4" s="1">
-        <v>44035.33841412037</v>
+        <v>44041.47287704861</v>
       </c>
       <c r="Z4">
-        <v>37</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5">
       <c r="A5">
-        <v>24</v>
+        <v>349</v>
       </c>
       <c r="B5">
         <v>12</v>
@@ -821,7 +821,7 @@
         <v>0</v>
       </c>
       <c r="T5">
-        <v>0.0172</v>
+        <v>0.01723</v>
       </c>
       <c r="U5">
         <v>0</v>
@@ -836,15 +836,15 @@
         <v>0</v>
       </c>
       <c r="Y5" s="1">
-        <v>44035.338519247685</v>
+        <v>44041.472987650464</v>
       </c>
       <c r="Z5">
-        <v>37</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6">
       <c r="A6">
-        <v>25</v>
+        <v>350</v>
       </c>
       <c r="B6">
         <v>13</v>
@@ -916,15 +916,15 @@
         <v>0</v>
       </c>
       <c r="Y6" s="1">
-        <v>44035.338616284724</v>
+        <v>44041.4730900463</v>
       </c>
       <c r="Z6">
-        <v>37</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7">
       <c r="A7">
-        <v>26</v>
+        <v>351</v>
       </c>
       <c r="B7">
         <v>14</v>
@@ -984,7 +984,7 @@
         <v>0</v>
       </c>
       <c r="U7">
-        <v>2.98939</v>
+        <v>2.98841</v>
       </c>
       <c r="V7">
         <v>0</v>
@@ -996,15 +996,15 @@
         <v>0</v>
       </c>
       <c r="Y7" s="1">
-        <v>44035.33874236111</v>
+        <v>44041.47321643519</v>
       </c>
       <c r="Z7">
-        <v>37</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8">
       <c r="A8">
-        <v>27</v>
+        <v>352</v>
       </c>
       <c r="B8">
         <v>15</v>
@@ -1064,7 +1064,7 @@
         <v>0</v>
       </c>
       <c r="U8">
-        <v>1.5017</v>
+        <v>1.50098</v>
       </c>
       <c r="V8">
         <v>0</v>
@@ -1076,15 +1076,15 @@
         <v>0</v>
       </c>
       <c r="Y8" s="1">
-        <v>44035.33885277778</v>
+        <v>44041.47332596065</v>
       </c>
       <c r="Z8">
-        <v>37</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9">
       <c r="A9">
-        <v>28</v>
+        <v>353</v>
       </c>
       <c r="B9">
         <v>16</v>
@@ -1144,7 +1144,7 @@
         <v>0</v>
       </c>
       <c r="U9">
-        <v>0.30049</v>
+        <v>0.30014</v>
       </c>
       <c r="V9">
         <v>0</v>
@@ -1156,15 +1156,15 @@
         <v>0</v>
       </c>
       <c r="Y9" s="1">
-        <v>44035.33895251157</v>
+        <v>44041.47342638889</v>
       </c>
       <c r="Z9">
-        <v>37</v>
+        <v>56</v>
       </c>
     </row>
     <row r="10">
       <c r="A10">
-        <v>29</v>
+        <v>354</v>
       </c>
       <c r="B10">
         <v>17</v>
@@ -1224,7 +1224,7 @@
         <v>0</v>
       </c>
       <c r="U10">
-        <v>0.07993</v>
+        <v>0.08002</v>
       </c>
       <c r="V10">
         <v>0</v>
@@ -1236,15 +1236,15 @@
         <v>0</v>
       </c>
       <c r="Y10" s="1">
-        <v>44035.339062534724</v>
+        <v>44041.47353634259</v>
       </c>
       <c r="Z10">
-        <v>37</v>
+        <v>56</v>
       </c>
     </row>
     <row r="11">
       <c r="A11">
-        <v>30</v>
+        <v>355</v>
       </c>
       <c r="B11">
         <v>18</v>
@@ -1316,15 +1316,15 @@
         <v>0</v>
       </c>
       <c r="Y11" s="1">
-        <v>44035.339164351855</v>
+        <v>44041.473637696756</v>
       </c>
       <c r="Z11">
-        <v>37</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12">
       <c r="A12">
-        <v>31</v>
+        <v>356</v>
       </c>
       <c r="B12">
         <v>19</v>
@@ -1387,7 +1387,7 @@
         <v>0</v>
       </c>
       <c r="V12">
-        <v>2.97425</v>
+        <v>2.97702</v>
       </c>
       <c r="W12">
         <v>0</v>
@@ -1396,15 +1396,15 @@
         <v>0</v>
       </c>
       <c r="Y12" s="1">
-        <v>44035.33928125</v>
+        <v>44041.47375428241</v>
       </c>
       <c r="Z12">
-        <v>37</v>
+        <v>56</v>
       </c>
     </row>
     <row r="13">
       <c r="A13">
-        <v>32</v>
+        <v>357</v>
       </c>
       <c r="B13">
         <v>20</v>
@@ -1467,7 +1467,7 @@
         <v>0</v>
       </c>
       <c r="V13">
-        <v>1.17939</v>
+        <v>1.17892</v>
       </c>
       <c r="W13">
         <v>0</v>
@@ -1476,15 +1476,15 @@
         <v>0</v>
       </c>
       <c r="Y13" s="1">
-        <v>44035.33939100694</v>
+        <v>44041.47386388889</v>
       </c>
       <c r="Z13">
-        <v>37</v>
+        <v>56</v>
       </c>
     </row>
     <row r="14">
       <c r="A14">
-        <v>33</v>
+        <v>358</v>
       </c>
       <c r="B14">
         <v>21</v>
@@ -1547,7 +1547,7 @@
         <v>0</v>
       </c>
       <c r="V14">
-        <v>0.09268</v>
+        <v>0.09261</v>
       </c>
       <c r="W14">
         <v>0</v>
@@ -1556,15 +1556,15 @@
         <v>0</v>
       </c>
       <c r="Y14" s="1">
-        <v>44035.33949209491</v>
+        <v>44041.47396458333</v>
       </c>
       <c r="Z14">
-        <v>37</v>
+        <v>56</v>
       </c>
     </row>
     <row r="15">
       <c r="A15">
-        <v>34</v>
+        <v>359</v>
       </c>
       <c r="B15">
         <v>22</v>
@@ -1627,7 +1627,7 @@
         <v>0</v>
       </c>
       <c r="V15">
-        <v>0.02498</v>
+        <v>0.02497</v>
       </c>
       <c r="W15">
         <v>0</v>
@@ -1636,15 +1636,15 @@
         <v>0</v>
       </c>
       <c r="Y15" s="1">
-        <v>44035.339593020835</v>
+        <v>44041.47406550926</v>
       </c>
       <c r="Z15">
-        <v>37</v>
+        <v>56</v>
       </c>
     </row>
     <row r="16">
       <c r="A16">
-        <v>35</v>
+        <v>360</v>
       </c>
       <c r="B16">
         <v>23</v>
@@ -1716,15 +1716,15 @@
         <v>0</v>
       </c>
       <c r="Y16" s="1">
-        <v>44035.33970462963</v>
+        <v>44041.47417581019</v>
       </c>
       <c r="Z16">
-        <v>37</v>
+        <v>56</v>
       </c>
     </row>
     <row r="17">
       <c r="A17">
-        <v>36</v>
+        <v>361</v>
       </c>
       <c r="B17">
         <v>24</v>
@@ -1790,21 +1790,21 @@
         <v>0</v>
       </c>
       <c r="W17">
-        <v>2.87611</v>
+        <v>2.87782</v>
       </c>
       <c r="X17" t="b">
         <v>0</v>
       </c>
       <c r="Y17" s="1">
-        <v>44035.33982947917</v>
+        <v>44041.47430158565</v>
       </c>
       <c r="Z17">
-        <v>37</v>
+        <v>56</v>
       </c>
     </row>
     <row r="18">
       <c r="A18">
-        <v>37</v>
+        <v>362</v>
       </c>
       <c r="B18">
         <v>25</v>
@@ -1870,21 +1870,21 @@
         <v>0</v>
       </c>
       <c r="W18">
-        <v>1.23918</v>
+        <v>1.24021</v>
       </c>
       <c r="X18" t="b">
         <v>0</v>
       </c>
       <c r="Y18" s="1">
-        <v>44035.33993862269</v>
+        <v>44041.47441096065</v>
       </c>
       <c r="Z18">
-        <v>37</v>
+        <v>56</v>
       </c>
     </row>
     <row r="19">
       <c r="A19">
-        <v>38</v>
+        <v>363</v>
       </c>
       <c r="B19">
         <v>26</v>
@@ -1950,21 +1950,21 @@
         <v>0</v>
       </c>
       <c r="W19">
-        <v>0.10657</v>
+        <v>0.10708</v>
       </c>
       <c r="X19" t="b">
         <v>0</v>
       </c>
       <c r="Y19" s="1">
-        <v>44035.340038773145</v>
+        <v>44041.47451184028</v>
       </c>
       <c r="Z19">
-        <v>37</v>
+        <v>56</v>
       </c>
     </row>
     <row r="20">
       <c r="A20">
-        <v>39</v>
+        <v>364</v>
       </c>
       <c r="B20">
         <v>27</v>
@@ -2030,21 +2030,21 @@
         <v>0</v>
       </c>
       <c r="W20">
-        <v>0.02997</v>
+        <v>0.0299</v>
       </c>
       <c r="X20" t="b">
         <v>0</v>
       </c>
       <c r="Y20" s="1">
-        <v>44035.34013938657</v>
+        <v>44041.474612997685</v>
       </c>
       <c r="Z20">
-        <v>37</v>
+        <v>56</v>
       </c>
     </row>
     <row r="21">
       <c r="A21">
-        <v>40</v>
+        <v>365</v>
       </c>
       <c r="B21">
         <v>28</v>
@@ -2116,10 +2116,10 @@
         <v>0</v>
       </c>
       <c r="Y21" s="1">
-        <v>44035.34025023148</v>
+        <v>44041.47481605324</v>
       </c>
       <c r="Z21">
-        <v>37</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed export filename to testId + boardId
</commit_message>
<xml_diff>
--- a/Export.xlsx
+++ b/Export.xlsx
@@ -407,7 +407,7 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="B2">
         <v>15</v>
@@ -425,7 +425,7 @@
         <v>7151:31323334</v>
       </c>
       <c r="G2" s="1">
-        <v>44041.472538229165</v>
+        <v>44042.32261403935</v>
       </c>
     </row>
   </sheetData>
@@ -524,7 +524,7 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>346</v>
+        <v>446</v>
       </c>
       <c r="B2">
         <v>9</v>
@@ -581,7 +581,7 @@
         <v>0</v>
       </c>
       <c r="T2">
-        <v>3.39566</v>
+        <v>3.38546</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -596,15 +596,15 @@
         <v>0</v>
       </c>
       <c r="Y2" s="1">
-        <v>44041.47266554398</v>
+        <v>44042.32274178241</v>
       </c>
       <c r="Z2">
-        <v>56</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3">
       <c r="A3">
-        <v>347</v>
+        <v>447</v>
       </c>
       <c r="B3">
         <v>10</v>
@@ -661,7 +661,7 @@
         <v>0</v>
       </c>
       <c r="T3">
-        <v>1.2619</v>
+        <v>1.25649</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -676,15 +676,15 @@
         <v>0</v>
       </c>
       <c r="Y3" s="1">
-        <v>44041.47277565972</v>
+        <v>44042.32285135417</v>
       </c>
       <c r="Z3">
-        <v>56</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4">
       <c r="A4">
-        <v>348</v>
+        <v>448</v>
       </c>
       <c r="B4">
         <v>11</v>
@@ -741,7 +741,7 @@
         <v>0</v>
       </c>
       <c r="T4">
-        <v>0.05568</v>
+        <v>0.05478</v>
       </c>
       <c r="U4">
         <v>0</v>
@@ -756,15 +756,15 @@
         <v>0</v>
       </c>
       <c r="Y4" s="1">
-        <v>44041.47287704861</v>
+        <v>44042.32295204861</v>
       </c>
       <c r="Z4">
-        <v>56</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5">
       <c r="A5">
-        <v>349</v>
+        <v>449</v>
       </c>
       <c r="B5">
         <v>12</v>
@@ -821,7 +821,7 @@
         <v>0</v>
       </c>
       <c r="T5">
-        <v>0.01723</v>
+        <v>0.01692</v>
       </c>
       <c r="U5">
         <v>0</v>
@@ -836,15 +836,15 @@
         <v>0</v>
       </c>
       <c r="Y5" s="1">
-        <v>44041.472987650464</v>
+        <v>44042.323061689814</v>
       </c>
       <c r="Z5">
-        <v>56</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6">
       <c r="A6">
-        <v>350</v>
+        <v>450</v>
       </c>
       <c r="B6">
         <v>13</v>
@@ -916,15 +916,15 @@
         <v>0</v>
       </c>
       <c r="Y6" s="1">
-        <v>44041.4730900463</v>
+        <v>44042.32316165509</v>
       </c>
       <c r="Z6">
-        <v>56</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7">
       <c r="A7">
-        <v>351</v>
+        <v>451</v>
       </c>
       <c r="B7">
         <v>14</v>
@@ -984,7 +984,7 @@
         <v>0</v>
       </c>
       <c r="U7">
-        <v>2.98841</v>
+        <v>2.98076</v>
       </c>
       <c r="V7">
         <v>0</v>
@@ -996,15 +996,15 @@
         <v>0</v>
       </c>
       <c r="Y7" s="1">
-        <v>44041.47321643519</v>
+        <v>44042.323287928244</v>
       </c>
       <c r="Z7">
-        <v>56</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8">
       <c r="A8">
-        <v>352</v>
+        <v>452</v>
       </c>
       <c r="B8">
         <v>15</v>
@@ -1064,7 +1064,7 @@
         <v>0</v>
       </c>
       <c r="U8">
-        <v>1.50098</v>
+        <v>1.49365</v>
       </c>
       <c r="V8">
         <v>0</v>
@@ -1076,15 +1076,15 @@
         <v>0</v>
       </c>
       <c r="Y8" s="1">
-        <v>44041.47332596065</v>
+        <v>44042.32339849537</v>
       </c>
       <c r="Z8">
-        <v>56</v>
+        <v>61</v>
       </c>
     </row>
     <row r="9">
       <c r="A9">
-        <v>353</v>
+        <v>453</v>
       </c>
       <c r="B9">
         <v>16</v>
@@ -1144,7 +1144,7 @@
         <v>0</v>
       </c>
       <c r="U9">
-        <v>0.30014</v>
+        <v>0.29824</v>
       </c>
       <c r="V9">
         <v>0</v>
@@ -1156,15 +1156,15 @@
         <v>0</v>
       </c>
       <c r="Y9" s="1">
-        <v>44041.47342638889</v>
+        <v>44042.32349927083</v>
       </c>
       <c r="Z9">
-        <v>56</v>
+        <v>61</v>
       </c>
     </row>
     <row r="10">
       <c r="A10">
-        <v>354</v>
+        <v>454</v>
       </c>
       <c r="B10">
         <v>17</v>
@@ -1224,7 +1224,7 @@
         <v>0</v>
       </c>
       <c r="U10">
-        <v>0.08002</v>
+        <v>0.07969</v>
       </c>
       <c r="V10">
         <v>0</v>
@@ -1236,15 +1236,15 @@
         <v>0</v>
       </c>
       <c r="Y10" s="1">
-        <v>44041.47353634259</v>
+        <v>44042.32360899306</v>
       </c>
       <c r="Z10">
-        <v>56</v>
+        <v>61</v>
       </c>
     </row>
     <row r="11">
       <c r="A11">
-        <v>355</v>
+        <v>455</v>
       </c>
       <c r="B11">
         <v>18</v>
@@ -1304,7 +1304,7 @@
         <v>0</v>
       </c>
       <c r="U11">
-        <v>0.00087</v>
+        <v>0.00086</v>
       </c>
       <c r="V11">
         <v>0</v>
@@ -1316,15 +1316,15 @@
         <v>0</v>
       </c>
       <c r="Y11" s="1">
-        <v>44041.473637696756</v>
+        <v>44042.323708993055</v>
       </c>
       <c r="Z11">
-        <v>56</v>
+        <v>61</v>
       </c>
     </row>
     <row r="12">
       <c r="A12">
-        <v>356</v>
+        <v>456</v>
       </c>
       <c r="B12">
         <v>19</v>
@@ -1387,7 +1387,7 @@
         <v>0</v>
       </c>
       <c r="V12">
-        <v>2.97702</v>
+        <v>2.9905</v>
       </c>
       <c r="W12">
         <v>0</v>
@@ -1396,15 +1396,15 @@
         <v>0</v>
       </c>
       <c r="Y12" s="1">
-        <v>44041.47375428241</v>
+        <v>44042.32382549768</v>
       </c>
       <c r="Z12">
-        <v>56</v>
+        <v>61</v>
       </c>
     </row>
     <row r="13">
       <c r="A13">
-        <v>357</v>
+        <v>457</v>
       </c>
       <c r="B13">
         <v>20</v>
@@ -1467,7 +1467,7 @@
         <v>0</v>
       </c>
       <c r="V13">
-        <v>1.17892</v>
+        <v>1.17426</v>
       </c>
       <c r="W13">
         <v>0</v>
@@ -1476,15 +1476,15 @@
         <v>0</v>
       </c>
       <c r="Y13" s="1">
-        <v>44041.47386388889</v>
+        <v>44042.32393503472</v>
       </c>
       <c r="Z13">
-        <v>56</v>
+        <v>61</v>
       </c>
     </row>
     <row r="14">
       <c r="A14">
-        <v>358</v>
+        <v>458</v>
       </c>
       <c r="B14">
         <v>21</v>
@@ -1547,7 +1547,7 @@
         <v>0</v>
       </c>
       <c r="V14">
-        <v>0.09261</v>
+        <v>0.09117</v>
       </c>
       <c r="W14">
         <v>0</v>
@@ -1556,15 +1556,15 @@
         <v>0</v>
       </c>
       <c r="Y14" s="1">
-        <v>44041.47396458333</v>
+        <v>44042.32403521991</v>
       </c>
       <c r="Z14">
-        <v>56</v>
+        <v>61</v>
       </c>
     </row>
     <row r="15">
       <c r="A15">
-        <v>359</v>
+        <v>459</v>
       </c>
       <c r="B15">
         <v>22</v>
@@ -1627,7 +1627,7 @@
         <v>0</v>
       </c>
       <c r="V15">
-        <v>0.02497</v>
+        <v>0.02457</v>
       </c>
       <c r="W15">
         <v>0</v>
@@ -1636,15 +1636,15 @@
         <v>0</v>
       </c>
       <c r="Y15" s="1">
-        <v>44041.47406550926</v>
+        <v>44042.32413587963</v>
       </c>
       <c r="Z15">
-        <v>56</v>
+        <v>61</v>
       </c>
     </row>
     <row r="16">
       <c r="A16">
-        <v>360</v>
+        <v>460</v>
       </c>
       <c r="B16">
         <v>23</v>
@@ -1707,7 +1707,7 @@
         <v>0</v>
       </c>
       <c r="V16">
-        <v>0.00046</v>
+        <v>0.00045</v>
       </c>
       <c r="W16">
         <v>0</v>
@@ -1716,15 +1716,15 @@
         <v>0</v>
       </c>
       <c r="Y16" s="1">
-        <v>44041.47417581019</v>
+        <v>44042.324246412034</v>
       </c>
       <c r="Z16">
-        <v>56</v>
+        <v>61</v>
       </c>
     </row>
     <row r="17">
       <c r="A17">
-        <v>361</v>
+        <v>461</v>
       </c>
       <c r="B17">
         <v>24</v>
@@ -1790,21 +1790,21 @@
         <v>0</v>
       </c>
       <c r="W17">
-        <v>2.87782</v>
+        <v>2.86945</v>
       </c>
       <c r="X17" t="b">
         <v>0</v>
       </c>
       <c r="Y17" s="1">
-        <v>44041.47430158565</v>
+        <v>44042.324371759256</v>
       </c>
       <c r="Z17">
-        <v>56</v>
+        <v>61</v>
       </c>
     </row>
     <row r="18">
       <c r="A18">
-        <v>362</v>
+        <v>462</v>
       </c>
       <c r="B18">
         <v>25</v>
@@ -1870,21 +1870,21 @@
         <v>0</v>
       </c>
       <c r="W18">
-        <v>1.24021</v>
+        <v>1.23445</v>
       </c>
       <c r="X18" t="b">
         <v>0</v>
       </c>
       <c r="Y18" s="1">
-        <v>44041.47441096065</v>
+        <v>44042.32448113426</v>
       </c>
       <c r="Z18">
-        <v>56</v>
+        <v>61</v>
       </c>
     </row>
     <row r="19">
       <c r="A19">
-        <v>363</v>
+        <v>463</v>
       </c>
       <c r="B19">
         <v>26</v>
@@ -1950,21 +1950,21 @@
         <v>0</v>
       </c>
       <c r="W19">
-        <v>0.10708</v>
+        <v>0.10529</v>
       </c>
       <c r="X19" t="b">
         <v>0</v>
       </c>
       <c r="Y19" s="1">
-        <v>44041.47451184028</v>
+        <v>44042.324581863424</v>
       </c>
       <c r="Z19">
-        <v>56</v>
+        <v>61</v>
       </c>
     </row>
     <row r="20">
       <c r="A20">
-        <v>364</v>
+        <v>464</v>
       </c>
       <c r="B20">
         <v>27</v>
@@ -2030,21 +2030,21 @@
         <v>0</v>
       </c>
       <c r="W20">
-        <v>0.0299</v>
+        <v>0.02899</v>
       </c>
       <c r="X20" t="b">
         <v>0</v>
       </c>
       <c r="Y20" s="1">
-        <v>44041.474612997685</v>
+        <v>44042.32468194445</v>
       </c>
       <c r="Z20">
-        <v>56</v>
+        <v>61</v>
       </c>
     </row>
     <row r="21">
       <c r="A21">
-        <v>365</v>
+        <v>465</v>
       </c>
       <c r="B21">
         <v>28</v>
@@ -2110,16 +2110,16 @@
         <v>0</v>
       </c>
       <c r="W21">
-        <v>0.00039</v>
+        <v>0.0004</v>
       </c>
       <c r="X21" t="b">
         <v>0</v>
       </c>
       <c r="Y21" s="1">
-        <v>44041.47481605324</v>
+        <v>44042.32479293981</v>
       </c>
       <c r="Z21">
-        <v>56</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>